<commit_message>
Fix : ItemData 의 AttackPower가 AttackPoser에서 안바뀌는 문제 해결
돌 에셋도 추가
</commit_message>
<xml_diff>
--- a/ExcelDB/ItemSheet.xlsx
+++ b/ExcelDB/ItemSheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suyb1\Documents\GitHub\Survival\Survival\Assets\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suyb1\Documents\GitHub\Survival\ExcelDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D02D5C5-626A-4D76-B187-8AE7D4DEE3BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84276E91-880E-4602-AAC9-26F664F2A341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6915" yWindow="675" windowWidth="25710" windowHeight="14805" xr2:uid="{8724138D-4329-4049-9136-E46855B368F2}"/>
+    <workbookView xWindow="14400" yWindow="675" windowWidth="21090" windowHeight="14805" xr2:uid="{8724138D-4329-4049-9136-E46855B368F2}"/>
   </bookViews>
   <sheets>
     <sheet name="ItemData" sheetId="1" r:id="rId1"/>
@@ -58,207 +58,207 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Hunger</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Water</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BodyTemperture</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AttackPower</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MoveSpeed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JumpForce</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Duration</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SpritePath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PrefabPath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MaxQuantity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IsStackable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>랩터고기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스테고사우르스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파키케팔로사우루스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물입니다. 수분을 10 제공합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>랩터의 고기입니다. 허기를 10 제공합니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스테고사우르스의 고기입니다. 허기를 10 제공합니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파키케팔로사우루스의 고기입니다. 허기를 10 제공합니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>풀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>풀입니다. 먹을 순 있지만 맛은 없습니다. 허기를 1 제공합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나무</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>돌</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>돌입니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나무입니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메이스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">메이스 입니다. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>잘구운 랩터고기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>잘 구워진 랩터 고기입니다. 허기를 20 제공합니다. 체온을 1도 올려줍니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ItemPrefabs/101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ItemPrefabs/102</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ItemPrefabs/103</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ItemPrefabs/104</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ItemPrefabs/111</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ItemPrefabs/121</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ItemPrefabs/201</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ItemPrefabs/210</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ItemPrefabs/301</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Consumable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resource</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Weapon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprites/Item/101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprites/Item/102</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprites/Item/103</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprites/Item/104</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprites/Item/111</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprites/Item/121</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprites/Item/201</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprites/Item/202</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprites/Item/301</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Stamina</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hunger</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Water</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BodyTemperture</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AttackPower</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MoveSpeed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JumpForce</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Duration</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SpritePath</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PrefabPath</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MaxQuantity</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IsStackable</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>랩터고기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>스테고사우르스</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>파키케팔로사우루스</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>물</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>물입니다. 수분을 10 제공합니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>랩터의 고기입니다. 허기를 10 제공합니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>스테고사우르스의 고기입니다. 허기를 10 제공합니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>파키케팔로사우루스의 고기입니다. 허기를 10 제공합니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>풀</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>풀입니다. 먹을 순 있지만 맛은 없습니다. 허기를 1 제공합니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>나무</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>돌</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>돌입니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>나무입니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>메이스</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">메이스 입니다. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>잘구운 랩터고기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>잘 구워진 랩터 고기입니다. 허기를 20 제공합니다. 체온을 1도 올려줍니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ItemPrefabs/101</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ItemPrefabs/102</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ItemPrefabs/103</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ItemPrefabs/104</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ItemPrefabs/111</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ItemPrefabs/121</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ItemPrefabs/201</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ItemPrefabs/210</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ItemPrefabs/301</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Consumable</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Resource</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Weapon</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sprites/Item/101</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sprites/Item/102</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sprites/Item/103</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sprites/Item/104</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sprites/Item/111</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sprites/Item/121</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sprites/Item/201</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sprites/Item/202</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sprites/Item/301</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -646,7 +646,7 @@
   <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -671,40 +671,40 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
-        <v>15</v>
-      </c>
-      <c r="O1" t="s">
-        <v>16</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
@@ -712,13 +712,13 @@
         <v>101</v>
       </c>
       <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -754,10 +754,10 @@
         <v>1</v>
       </c>
       <c r="P2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
@@ -765,13 +765,13 @@
         <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -807,10 +807,10 @@
         <v>1</v>
       </c>
       <c r="P3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
@@ -818,13 +818,13 @@
         <v>103</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -860,10 +860,10 @@
         <v>1</v>
       </c>
       <c r="P4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Q4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
@@ -871,13 +871,13 @@
         <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -913,10 +913,10 @@
         <v>1</v>
       </c>
       <c r="P5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
@@ -924,13 +924,13 @@
         <v>111</v>
       </c>
       <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
         <v>25</v>
       </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -966,10 +966,10 @@
         <v>1</v>
       </c>
       <c r="P6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
@@ -977,13 +977,13 @@
         <v>121</v>
       </c>
       <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
         <v>33</v>
       </c>
-      <c r="C7" t="s">
-        <v>34</v>
-      </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -1019,10 +1019,10 @@
         <v>1</v>
       </c>
       <c r="P7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Q7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
@@ -1030,13 +1030,13 @@
         <v>201</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -1072,10 +1072,10 @@
         <v>1</v>
       </c>
       <c r="P8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
@@ -1083,13 +1083,13 @@
         <v>210</v>
       </c>
       <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
         <v>28</v>
       </c>
-      <c r="C9" t="s">
-        <v>29</v>
-      </c>
       <c r="D9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -1125,10 +1125,10 @@
         <v>1</v>
       </c>
       <c r="P9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
@@ -1136,13 +1136,13 @@
         <v>301</v>
       </c>
       <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
         <v>31</v>
       </c>
-      <c r="C10" t="s">
-        <v>32</v>
-      </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1178,10 +1178,10 @@
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>